<commit_message>
Discussed questions with Lukas
</commit_message>
<xml_diff>
--- a/TODOs Ontologie.xlsx
+++ b/TODOs Ontologie.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0FAA3178-6333-420B-9370-0E08619F5F28}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Fragen an Ivan" sheetId="1" r:id="rId1"/>
-    <sheet name="Fragen an Lukas" sheetId="2" r:id="rId2"/>
+    <sheet name="TODO" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Wie erhalte ich die Links für die Prefix</t>
   </si>
@@ -47,57 +46,24 @@
     <t>77-105</t>
   </si>
   <si>
-    <t>Habe meiste Translations und min/max - lenghts selbst definiert. Kontrolle? Langzeit Testing?</t>
-  </si>
-  <si>
     <t>Werden Listen-Properties richtig dargestellt?</t>
   </si>
   <si>
     <t>Wo werden Listen abgespeichert, wie werden die Links erstellt?</t>
   </si>
   <si>
-    <t xml:space="preserve">Umgebung Lage Situation. </t>
-  </si>
-  <si>
     <t>Werden Datums-Properties richtig dargestellt</t>
   </si>
   <si>
-    <t>Abhub übersetzung Refuse?</t>
-  </si>
-  <si>
-    <t>Schnitt/Quadrant übersetzig profile/quadrant</t>
-  </si>
-  <si>
-    <t>Position/Befundliste übersetzig Position/findingslist</t>
-  </si>
-  <si>
-    <t>KatalogAbbildung sollte wahrscheinlich ein Link zu Bild sein</t>
-  </si>
-  <si>
     <t xml:space="preserve">Was genau bedeutet dcterms? Was ist das für eine Datei? </t>
   </si>
   <si>
-    <t>z.b 952</t>
-  </si>
-  <si>
-    <t>Planum übersetzig Plane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raum übersetzig Space (odr sottis room si ) </t>
-  </si>
-  <si>
-    <t>positionDarueber/Darunter links uf Position?</t>
-  </si>
-  <si>
     <t>PublikationNr lösche?</t>
   </si>
   <si>
     <t xml:space="preserve">Gibt es Hyperlink-Properties? </t>
   </si>
   <si>
-    <t xml:space="preserve">Befund Vergesellschaftung Übersetzig? </t>
-  </si>
-  <si>
     <t>Gibt es binäre Properties?</t>
   </si>
   <si>
@@ -134,13 +100,49 @@
     <t>Hat Zeichnung ein Bild?</t>
   </si>
   <si>
-    <t>Analysen/Restaurierung Klasse?</t>
+    <t xml:space="preserve">Findings </t>
+  </si>
+  <si>
+    <t>Finds</t>
+  </si>
+  <si>
+    <t>Schnitt/Quadrant übersetzig section</t>
+  </si>
+  <si>
+    <t>Raum</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>positionDarueber/Darunter links uf Position</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>Nein</t>
+  </si>
+  <si>
+    <t>Plan auch StillImageRepresentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lage alles 0-1 und denne mehreri Lage Objekt, Lage nur für d Abkürzig vom ganze, wie verlinke? -&gt; Ivan </t>
+  </si>
+  <si>
+    <t>Jpeg 2000 conversion 1000 bilder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lage Situation besprechen </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -150,18 +152,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -176,13 +172,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -452,21 +447,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="101.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
@@ -519,7 +514,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>144</v>
@@ -527,7 +522,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>145</v>
@@ -535,7 +530,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>236</v>
@@ -543,12 +538,12 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>1817</v>
@@ -556,7 +551,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>2601</v>
@@ -564,7 +559,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>2724</v>
@@ -572,17 +567,22 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -592,144 +592,115 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5964120B-45B3-4803-B2DF-F2CA31108A08}">
-  <dimension ref="A1:B19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="85.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="94.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>16</v>
-      </c>
-      <c r="B6">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8">
-        <v>1340</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9">
-        <v>1410</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10">
-        <v>1690</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12">
-        <v>2701</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>27</v>
       </c>
       <c r="B13">
         <v>2705</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Handled all TODOs until meeting with Lukas Ro
</commit_message>
<xml_diff>
--- a/TODOs Ontologie.xlsx
+++ b/TODOs Ontologie.xlsx
@@ -4,11 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Fragen an Ivan" sheetId="1" r:id="rId1"/>
-    <sheet name="TODO" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Wie erhalte ich die Links für die Prefix</t>
   </si>
@@ -58,27 +57,15 @@
     <t xml:space="preserve">Was genau bedeutet dcterms? Was ist das für eine Datei? </t>
   </si>
   <si>
-    <t>PublikationNr lösche?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gibt es Hyperlink-Properties? </t>
   </si>
   <si>
     <t>Gibt es binäre Properties?</t>
   </si>
   <si>
-    <t xml:space="preserve">Sollten alle Vasen als Gefaesse bezeichnet werden? </t>
-  </si>
-  <si>
-    <t>Persoenlichkeit-MaskenNr?</t>
-  </si>
-  <si>
     <t>Für 0-n wird wohl keine Kardinalitätsangabe benötigt?</t>
   </si>
   <si>
-    <t>Bilder für Klassen?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Für was werden die Kommentare der einzelnen Klassen benutzt? </t>
   </si>
   <si>
@@ -88,55 +75,16 @@
     <t>Gibt es mehr typen ausser Resource und StillImageRepresentation?</t>
   </si>
   <si>
-    <t>Bild-Kartonage Nr?</t>
-  </si>
-  <si>
-    <t>Plan-Kampagne?</t>
-  </si>
-  <si>
-    <t>Tagebuch-Abhub?</t>
-  </si>
-  <si>
-    <t>Hat Zeichnung ein Bild?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Findings </t>
-  </si>
-  <si>
-    <t>Finds</t>
-  </si>
-  <si>
-    <t>Schnitt/Quadrant übersetzig section</t>
-  </si>
-  <si>
-    <t>Raum</t>
-  </si>
-  <si>
-    <t>Room</t>
-  </si>
-  <si>
-    <t>positionDarueber/Darunter links uf Position</t>
-  </si>
-  <si>
-    <t>Ja</t>
-  </si>
-  <si>
-    <t>Delete</t>
-  </si>
-  <si>
-    <t>Nein</t>
-  </si>
-  <si>
-    <t>Plan auch StillImageRepresentation</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lage alles 0-1 und denne mehreri Lage Objekt, Lage nur für d Abkürzig vom ganze, wie verlinke? -&gt; Ivan </t>
   </si>
   <si>
-    <t>Jpeg 2000 conversion 1000 bilder</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lage Situation besprechen </t>
+  </si>
+  <si>
+    <t>Richtig, dass Zeichnung und Plan StillImageRepresentation? Auch wenn PDF?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sollten min und max überhaupt definiert werden? </t>
   </si>
 </sst>
 </file>
@@ -455,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,7 +491,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>1817</v>
@@ -551,7 +499,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>2601</v>
@@ -559,7 +507,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>2724</v>
@@ -567,140 +515,41 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="94.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6">
-        <v>1690</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13">
-        <v>2705</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>